<commit_message>
perdhesa e kateve done
</commit_message>
<xml_diff>
--- a/3-Katet/regjistri/29-Koordinatat-e-kateve-Dior.xlsx
+++ b/3-Katet/regjistri/29-Koordinatat-e-kateve-Dior.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Ferizaj\Ferizaj\Ingjinierike\565-6-Shefkia1\3-Katet\regjistri\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Ferizaj\Sojevë\INXHINIERIKE\Dior\3-Katet\regjistri\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$78</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$88</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="36">
   <si>
     <t>Y</t>
   </si>
@@ -72,21 +72,6 @@
     <t>Sead Prushi</t>
   </si>
   <si>
-    <t>O1-1</t>
-  </si>
-  <si>
-    <t>O1-2</t>
-  </si>
-  <si>
-    <t>O1-3</t>
-  </si>
-  <si>
-    <t>O1-4</t>
-  </si>
-  <si>
-    <t>SHKALLET</t>
-  </si>
-  <si>
     <t>Sqarim</t>
   </si>
   <si>
@@ -154,6 +139,12 @@
   </si>
   <si>
     <t>Nënkulm</t>
+  </si>
+  <si>
+    <t>PERDHESA</t>
+  </si>
+  <si>
+    <t>SHKALET</t>
   </si>
 </sst>
 </file>
@@ -201,7 +192,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -623,30 +614,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -659,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -720,10 +687,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -741,16 +708,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -760,6 +727,54 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -820,62 +835,11 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1515,10 +1479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K81"/>
+  <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A52" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37:F44"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1534,115 +1498,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
     </row>
     <row r="2" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
+      <c r="A4" s="60"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
+      <c r="A5" s="60"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
+      <c r="A6" s="60"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="63"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="65"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="48"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="66"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="68"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="51"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="69"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="70"/>
-      <c r="H10" s="70"/>
-      <c r="I10" s="70"/>
-      <c r="J10" s="71"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="54"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
@@ -1664,16 +1628,16 @@
         <v>1</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>6</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I14" s="12" t="s">
         <v>7</v>
@@ -1681,574 +1645,563 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="13">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C15" s="5">
-        <v>7510843.9336000001</v>
+        <v>7517924.0990000004</v>
       </c>
       <c r="D15" s="5">
-        <v>4693754.3136</v>
+        <v>4692685.9060000004</v>
       </c>
       <c r="E15" s="16">
-        <v>580.96799999999996</v>
+        <v>616.38300000000004</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="72" t="s">
+      <c r="H15" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="75">
+      <c r="I15" s="40">
         <v>208.47</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="13">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C16" s="5">
-        <v>7510835.4665000001</v>
+        <v>7517928.4419999998</v>
       </c>
       <c r="D16" s="5">
-        <v>4693745.7829</v>
+        <v>4692673.07</v>
       </c>
       <c r="E16" s="16">
-        <v>580.96799999999996</v>
+        <v>616.38300000000004</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="73"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="76"/>
+        <v>34</v>
+      </c>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="13">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C17" s="5">
-        <v>7510831.7971999999</v>
+        <v>7517929.8169999998</v>
       </c>
       <c r="D17" s="5">
-        <v>4693766.6201999998</v>
+        <v>4692673.5259999996</v>
       </c>
       <c r="E17" s="16">
-        <v>580.96799999999996</v>
+        <v>616.38300000000004</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="73"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="76"/>
+        <v>34</v>
+      </c>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="13">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="C18" s="5">
-        <v>7510823.2538000001</v>
+        <v>7517929.96</v>
       </c>
       <c r="D18" s="5">
-        <v>4693758.1205000002</v>
+        <v>4692673.2819999997</v>
       </c>
       <c r="E18" s="16">
-        <v>580.96799999999996</v>
+        <v>616.38300000000004</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="73"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="77"/>
+        <v>34</v>
+      </c>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="13">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="C19" s="5">
-        <v>7510826.4108999996</v>
+        <v>7517930.2989999996</v>
       </c>
       <c r="D19" s="5">
-        <v>4693754.9310999997</v>
+        <v>4692672.9689999996</v>
       </c>
       <c r="E19" s="16">
-        <v>580.96799999999996</v>
+        <v>616.38300000000004</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="73"/>
-      <c r="H19" s="72" t="s">
-        <v>19</v>
-      </c>
-      <c r="I19" s="75">
-        <v>9.24</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="13">
-        <v>97</v>
+        <v>9</v>
       </c>
       <c r="C20" s="5">
-        <v>7510825.6070999997</v>
+        <v>7517930.7450000001</v>
       </c>
       <c r="D20" s="5">
-        <v>4693754.1304000001</v>
+        <v>4692672.7690000003</v>
       </c>
       <c r="E20" s="16">
-        <v>580.96799999999996</v>
+        <v>616.38300000000004</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="73"/>
-      <c r="H20" s="73"/>
-      <c r="I20" s="76"/>
+        <v>34</v>
+      </c>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="13">
-        <v>98</v>
+        <v>10</v>
       </c>
       <c r="C21" s="5">
-        <v>7510831.4223999996</v>
+        <v>7517931.2220000001</v>
       </c>
       <c r="D21" s="5">
-        <v>4693748.2926000003</v>
+        <v>4692672.7319999998</v>
       </c>
       <c r="E21" s="16">
-        <v>580.96799999999996</v>
+        <v>616.38300000000004</v>
       </c>
       <c r="F21" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="13">
+        <v>11</v>
+      </c>
+      <c r="C22" s="5">
+        <v>7517931.6050000004</v>
+      </c>
+      <c r="D22" s="5">
+        <v>4692672.7970000003</v>
+      </c>
+      <c r="E22" s="16">
+        <v>616.38300000000004</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="13">
+        <v>34</v>
+      </c>
+      <c r="C23" s="5">
+        <v>7517953.7189999996</v>
+      </c>
+      <c r="D23" s="5">
+        <v>4692687.3470000001</v>
+      </c>
+      <c r="E23" s="16">
+        <v>616.38300000000004</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="13">
+        <v>35</v>
+      </c>
+      <c r="C24" s="5">
+        <v>7517955.8949999996</v>
+      </c>
+      <c r="D24" s="5">
+        <v>4692681.023</v>
+      </c>
+      <c r="E24" s="16">
+        <v>616.38300000000004</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="13">
+        <v>58</v>
+      </c>
+      <c r="C25" s="5">
+        <v>7517951.3300000001</v>
+      </c>
+      <c r="D25" s="5">
+        <v>4692686.5060000001</v>
+      </c>
+      <c r="E25" s="16">
+        <v>616.38300000000004</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="13">
+        <v>59</v>
+      </c>
+      <c r="C26" s="5">
+        <v>7517951.9790000003</v>
+      </c>
+      <c r="D26" s="5">
+        <v>4692687.1399999997</v>
+      </c>
+      <c r="E26" s="16">
+        <v>616.38300000000004</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="13">
+        <v>60</v>
+      </c>
+      <c r="C27" s="5">
+        <v>7517952.0760000004</v>
+      </c>
+      <c r="D27" s="5">
+        <v>4692688.1239999998</v>
+      </c>
+      <c r="E27" s="16">
+        <v>616.38300000000004</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="13">
+        <v>61</v>
+      </c>
+      <c r="C28" s="5">
+        <v>7517950.1849999996</v>
+      </c>
+      <c r="D28" s="5">
+        <v>4692693.4919999996</v>
+      </c>
+      <c r="E28" s="16">
+        <v>616.38300000000004</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="41"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="13">
+        <v>62</v>
+      </c>
+      <c r="C29" s="5">
+        <v>7517949.5559999999</v>
+      </c>
+      <c r="D29" s="5">
+        <v>4692694.1169999996</v>
+      </c>
+      <c r="E29" s="16">
+        <v>616.38300000000004</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="13">
+        <v>63</v>
+      </c>
+      <c r="C30" s="5">
+        <v>7517948.5300000003</v>
+      </c>
+      <c r="D30" s="5">
+        <v>4692694.1579999998</v>
+      </c>
+      <c r="E30" s="16">
+        <v>616.38300000000004</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" s="41"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="55"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="13">
+        <v>14</v>
+      </c>
+      <c r="C31" s="5">
+        <v>7517930.4069999997</v>
+      </c>
+      <c r="D31" s="5">
+        <v>4692671.8150000004</v>
+      </c>
+      <c r="E31" s="16">
+        <v>616.38300000000004</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" s="41"/>
+      <c r="H31" s="76" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="77">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="14">
         <v>15</v>
       </c>
-      <c r="G21" s="73"/>
-      <c r="H21" s="74"/>
-      <c r="I21" s="77"/>
-    </row>
-    <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="14">
-        <v>99</v>
-      </c>
-      <c r="C22" s="15">
-        <v>7510832.2077000001</v>
-      </c>
-      <c r="D22" s="15">
-        <v>4693749.0749000004</v>
-      </c>
-      <c r="E22" s="17">
-        <v>580.96799999999996</v>
-      </c>
-      <c r="F22" s="17" t="s">
+      <c r="C32" s="15">
+        <v>7517928.9910000004</v>
+      </c>
+      <c r="D32" s="15">
+        <v>4692671.3689999999</v>
+      </c>
+      <c r="E32" s="17">
+        <v>616.38300000000004</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" s="42"/>
+      <c r="H32" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="78"/>
-      <c r="H22" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I22" s="18">
-        <f>SUM(I15:I21)</f>
-        <v>217.71</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
+      <c r="I32" s="18">
+        <f>SUM(I15:I31)</f>
+        <v>226.95000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="6"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C34" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D34" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E34" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="23">
+        <v>7</v>
+      </c>
+      <c r="C35" s="19">
+        <v>7510827.4069999997</v>
+      </c>
+      <c r="D35" s="20">
+        <v>4693753.9248000002</v>
+      </c>
+      <c r="E35" s="5">
+        <v>584.09</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H24" s="11" t="s">
+      <c r="H35" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="I35" s="24">
+        <v>224.06</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="23">
+        <v>12</v>
+      </c>
+      <c r="C36" s="19">
+        <v>7510843.9336000001</v>
+      </c>
+      <c r="D36" s="20">
+        <v>4693754.3136</v>
+      </c>
+      <c r="E36" s="5">
+        <v>584.09</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I24" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="23">
-        <v>7</v>
-      </c>
-      <c r="C25" s="19">
-        <v>7510827.4069999997</v>
-      </c>
-      <c r="D25" s="20">
-        <v>4693753.9248000002</v>
-      </c>
-      <c r="E25" s="5">
-        <v>584.09</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G25" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="H25" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="I25" s="24">
-        <v>224.06</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="23">
-        <v>12</v>
-      </c>
-      <c r="C26" s="19">
-        <v>7510843.9336000001</v>
-      </c>
-      <c r="D26" s="20">
-        <v>4693754.3136</v>
-      </c>
-      <c r="E26" s="5">
-        <v>584.09</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="21"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="25"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="23">
-        <v>13</v>
-      </c>
-      <c r="C27" s="19">
-        <v>7510834.5436000004</v>
-      </c>
-      <c r="D27" s="20">
-        <v>4693744.8530999999</v>
-      </c>
-      <c r="E27" s="5">
-        <v>584.09</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="21"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="24"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="23">
-        <v>19</v>
-      </c>
-      <c r="C28" s="19">
-        <v>7510831.7971999999</v>
-      </c>
-      <c r="D28" s="20">
-        <v>4693766.6201999998</v>
-      </c>
-      <c r="E28" s="5">
-        <v>584.09</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G28" s="21"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="24"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="23">
-        <v>52</v>
-      </c>
-      <c r="C29" s="19">
-        <v>7510831.3317</v>
-      </c>
-      <c r="D29" s="20">
-        <v>4693749.9599000001</v>
-      </c>
-      <c r="E29" s="5">
-        <v>584.09</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G29" s="21"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="24"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="23">
-        <v>56</v>
-      </c>
-      <c r="C30" s="19">
-        <v>7510822.3073000005</v>
-      </c>
-      <c r="D30" s="20">
-        <v>4693757.1810999997</v>
-      </c>
-      <c r="E30" s="5">
-        <v>584.09</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G30" s="21"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="24"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="23">
-        <v>8</v>
-      </c>
-      <c r="C31" s="19">
-        <v>7510830.3949999996</v>
-      </c>
-      <c r="D31" s="20">
-        <v>4693749.0327000003</v>
-      </c>
-      <c r="E31" s="5">
-        <v>584.09</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G31" s="21"/>
-      <c r="H31" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="I31" s="24">
-        <v>20.72</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="23">
-        <v>100</v>
-      </c>
-      <c r="C32" s="19">
-        <v>7510826.4649999999</v>
-      </c>
-      <c r="D32" s="20">
-        <v>4693752.9923</v>
-      </c>
-      <c r="E32" s="5">
-        <v>584.09</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G32" s="21"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="24"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="23">
-        <v>101</v>
-      </c>
-      <c r="C33" s="19">
-        <v>7510832.6496000001</v>
-      </c>
-      <c r="D33" s="20">
-        <v>4693767.4611</v>
-      </c>
-      <c r="E33" s="5">
-        <v>584.09</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G33" s="21"/>
-      <c r="H33" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="I33" s="36">
-        <v>7.37</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="26">
-        <v>102</v>
-      </c>
-      <c r="C34" s="27">
-        <v>7510844.7790999999</v>
-      </c>
-      <c r="D34" s="28">
-        <v>4693755.1654000003</v>
-      </c>
-      <c r="E34" s="15">
-        <v>584.09</v>
-      </c>
-      <c r="F34" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G34" s="29"/>
-      <c r="H34" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I34" s="31">
-        <f>SUM(I25:I33)</f>
-        <v>252.15</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D35" s="6"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="12" t="s">
-        <v>7</v>
-      </c>
+      <c r="G36" s="21"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="25"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="23">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C37" s="19">
-        <v>7510823.2538000001</v>
+        <v>7510834.5436000004</v>
       </c>
       <c r="D37" s="20">
-        <v>4693758.1205000002</v>
+        <v>4693744.8530999999</v>
       </c>
       <c r="E37" s="5">
-        <v>587.16200000000003</v>
+        <v>584.09</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G37" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="H37" s="60" t="s">
-        <v>29</v>
-      </c>
-      <c r="I37" s="61">
-        <v>208.47</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G37" s="21"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="24"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="23">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C38" s="19">
-        <v>7510843.9336000001</v>
+        <v>7510831.7971999999</v>
       </c>
       <c r="D38" s="20">
-        <v>4693754.3136</v>
+        <v>4693766.6201999998</v>
       </c>
       <c r="E38" s="5">
-        <v>587.16200000000003</v>
+        <v>584.09</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G38" s="58"/>
-      <c r="H38" s="60"/>
-      <c r="I38" s="61"/>
+        <v>16</v>
+      </c>
+      <c r="G38" s="21"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="24"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="23">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="C39" s="19">
-        <v>7510835.4665000001</v>
+        <v>7510831.3317</v>
       </c>
       <c r="D39" s="20">
-        <v>4693745.7829</v>
+        <v>4693749.9599000001</v>
       </c>
       <c r="E39" s="5">
-        <v>587.16200000000003</v>
+        <v>584.09</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G39" s="58"/>
-      <c r="H39" s="60"/>
-      <c r="I39" s="61"/>
+        <v>16</v>
+      </c>
+      <c r="G39" s="21"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="24"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="23">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="C40" s="19">
-        <v>7510831.7971999999</v>
+        <v>7510822.3073000005</v>
       </c>
       <c r="D40" s="20">
-        <v>4693766.6201999998</v>
+        <v>4693757.1810999997</v>
       </c>
       <c r="E40" s="5">
-        <v>587.16200000000003</v>
+        <v>584.09</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G40" s="58"/>
-      <c r="H40" s="60"/>
-      <c r="I40" s="61"/>
+        <v>16</v>
+      </c>
+      <c r="G40" s="21"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="24"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="23">
         <v>8</v>
       </c>
       <c r="C41" s="19">
-        <v>7510834.5436000004</v>
+        <v>7510830.3949999996</v>
       </c>
       <c r="D41" s="20">
-        <v>4693744.8530999999</v>
+        <v>4693749.0327000003</v>
       </c>
       <c r="E41" s="5">
-        <v>587.16200000000003</v>
+        <v>584.09</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G41" s="58"/>
-      <c r="H41" s="60" t="s">
-        <v>25</v>
-      </c>
-      <c r="I41" s="61">
-        <v>22.95</v>
+        <v>17</v>
+      </c>
+      <c r="G41" s="21"/>
+      <c r="H41" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I41" s="24">
+        <v>20.72</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
@@ -2256,43 +2209,43 @@
         <v>100</v>
       </c>
       <c r="C42" s="19">
-        <v>7510822.3084000004</v>
+        <v>7510826.4649999999</v>
       </c>
       <c r="D42" s="20">
-        <v>4693757.18</v>
+        <v>4693752.9923</v>
       </c>
       <c r="E42" s="5">
-        <v>587.16200000000003</v>
+        <v>584.09</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G42" s="58"/>
-      <c r="H42" s="60"/>
-      <c r="I42" s="61"/>
+        <v>17</v>
+      </c>
+      <c r="G42" s="21"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="24"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="23">
         <v>101</v>
       </c>
       <c r="C43" s="19">
-        <v>7510832.6459999997</v>
+        <v>7510832.6496000001</v>
       </c>
       <c r="D43" s="20">
-        <v>4693767.4647000004</v>
+        <v>4693767.4611</v>
       </c>
       <c r="E43" s="5">
-        <v>587.16200000000003</v>
+        <v>584.09</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G43" s="58"/>
-      <c r="H43" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="I43" s="24">
-        <v>20.72</v>
+        <v>17</v>
+      </c>
+      <c r="G43" s="21"/>
+      <c r="H43" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="I43" s="36">
+        <v>7.37</v>
       </c>
     </row>
     <row r="44" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2306,18 +2259,18 @@
         <v>4693755.1654000003</v>
       </c>
       <c r="E44" s="15">
-        <v>587.16200000000003</v>
+        <v>584.09</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G44" s="59"/>
+        <v>17</v>
+      </c>
+      <c r="G44" s="29"/>
       <c r="H44" s="30" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="I44" s="31">
-        <f>SUM(I37:I43)</f>
-        <v>252.14</v>
+        <f>SUM(I35:I43)</f>
+        <v>252.15</v>
       </c>
     </row>
     <row r="45" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2339,16 +2292,16 @@
         <v>1</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G46" s="11" t="s">
         <v>6</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I46" s="12" t="s">
         <v>7</v>
@@ -2365,18 +2318,18 @@
         <v>4693758.1205000002</v>
       </c>
       <c r="E47" s="5">
-        <v>590.18700000000001</v>
+        <v>587.16200000000003</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G47" s="58" t="s">
-        <v>33</v>
-      </c>
-      <c r="H47" s="60" t="s">
-        <v>33</v>
-      </c>
-      <c r="I47" s="61">
+        <v>21</v>
+      </c>
+      <c r="G47" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="H47" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="I47" s="43">
         <v>208.47</v>
       </c>
     </row>
@@ -2391,14 +2344,14 @@
         <v>4693754.3136</v>
       </c>
       <c r="E48" s="5">
-        <v>590.18700000000001</v>
+        <v>587.16200000000003</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G48" s="58"/>
-      <c r="H48" s="60"/>
-      <c r="I48" s="61"/>
+        <v>21</v>
+      </c>
+      <c r="G48" s="74"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="43"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="23">
@@ -2411,14 +2364,14 @@
         <v>4693745.7829</v>
       </c>
       <c r="E49" s="5">
-        <v>590.18700000000001</v>
+        <v>587.16200000000003</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G49" s="58"/>
-      <c r="H49" s="60"/>
-      <c r="I49" s="61"/>
+        <v>21</v>
+      </c>
+      <c r="G49" s="74"/>
+      <c r="H49" s="44"/>
+      <c r="I49" s="43"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="23">
@@ -2431,14 +2384,14 @@
         <v>4693766.6201999998</v>
       </c>
       <c r="E50" s="5">
-        <v>590.18700000000001</v>
+        <v>587.16200000000003</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G50" s="58"/>
-      <c r="H50" s="60"/>
-      <c r="I50" s="61"/>
+        <v>21</v>
+      </c>
+      <c r="G50" s="74"/>
+      <c r="H50" s="44"/>
+      <c r="I50" s="43"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="23">
@@ -2451,16 +2404,16 @@
         <v>4693744.8530999999</v>
       </c>
       <c r="E51" s="5">
-        <v>590.18700000000001</v>
+        <v>587.16200000000003</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G51" s="58"/>
-      <c r="H51" s="60" t="s">
-        <v>25</v>
-      </c>
-      <c r="I51" s="61">
+        <v>22</v>
+      </c>
+      <c r="G51" s="74"/>
+      <c r="H51" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="I51" s="43">
         <v>22.95</v>
       </c>
     </row>
@@ -2475,14 +2428,14 @@
         <v>4693757.18</v>
       </c>
       <c r="E52" s="5">
-        <v>590.18700000000001</v>
+        <v>587.16200000000003</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G52" s="58"/>
-      <c r="H52" s="60"/>
-      <c r="I52" s="61"/>
+        <v>22</v>
+      </c>
+      <c r="G52" s="74"/>
+      <c r="H52" s="44"/>
+      <c r="I52" s="43"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="23">
@@ -2495,16 +2448,16 @@
         <v>4693767.4647000004</v>
       </c>
       <c r="E53" s="5">
-        <v>590.18700000000001</v>
+        <v>587.16200000000003</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G53" s="58"/>
-      <c r="H53" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="I53" s="33">
+        <v>22</v>
+      </c>
+      <c r="G53" s="74"/>
+      <c r="H53" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I53" s="24">
         <v>20.72</v>
       </c>
     </row>
@@ -2519,14 +2472,14 @@
         <v>4693755.1654000003</v>
       </c>
       <c r="E54" s="15">
-        <v>590.18700000000001</v>
+        <v>587.16200000000003</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G54" s="59"/>
+        <v>22</v>
+      </c>
+      <c r="G54" s="75"/>
       <c r="H54" s="30" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I54" s="31">
         <f>SUM(I47:I53)</f>
@@ -2552,16 +2505,16 @@
         <v>1</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G56" s="11" t="s">
         <v>6</v>
       </c>
       <c r="H56" s="11" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I56" s="12" t="s">
         <v>7</v>
@@ -2578,18 +2531,18 @@
         <v>4693758.1205000002</v>
       </c>
       <c r="E57" s="5">
-        <v>593.27200000000005</v>
+        <v>590.18700000000001</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G57" s="58" t="s">
-        <v>36</v>
-      </c>
-      <c r="H57" s="60" t="s">
-        <v>36</v>
-      </c>
-      <c r="I57" s="61">
+        <v>26</v>
+      </c>
+      <c r="G57" s="74" t="s">
+        <v>28</v>
+      </c>
+      <c r="H57" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="I57" s="43">
         <v>208.47</v>
       </c>
     </row>
@@ -2604,14 +2557,14 @@
         <v>4693754.3136</v>
       </c>
       <c r="E58" s="5">
-        <v>593.27200000000005</v>
+        <v>590.18700000000001</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G58" s="58"/>
-      <c r="H58" s="60"/>
-      <c r="I58" s="61"/>
+        <v>26</v>
+      </c>
+      <c r="G58" s="74"/>
+      <c r="H58" s="44"/>
+      <c r="I58" s="43"/>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="23">
@@ -2624,14 +2577,14 @@
         <v>4693745.7829</v>
       </c>
       <c r="E59" s="5">
-        <v>593.27200000000005</v>
+        <v>590.18700000000001</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G59" s="58"/>
-      <c r="H59" s="60"/>
-      <c r="I59" s="61"/>
+        <v>26</v>
+      </c>
+      <c r="G59" s="74"/>
+      <c r="H59" s="44"/>
+      <c r="I59" s="43"/>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="23">
@@ -2644,36 +2597,36 @@
         <v>4693766.6201999998</v>
       </c>
       <c r="E60" s="5">
-        <v>593.27200000000005</v>
+        <v>590.18700000000001</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G60" s="58"/>
-      <c r="H60" s="60"/>
-      <c r="I60" s="61"/>
+        <v>26</v>
+      </c>
+      <c r="G60" s="74"/>
+      <c r="H60" s="44"/>
+      <c r="I60" s="43"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="23">
         <v>8</v>
       </c>
       <c r="C61" s="19">
-        <v>7510834.5362</v>
+        <v>7510834.5436000004</v>
       </c>
       <c r="D61" s="20">
-        <v>4693744.8603999997</v>
+        <v>4693744.8530999999</v>
       </c>
       <c r="E61" s="5">
-        <v>593.27200000000005</v>
+        <v>590.18700000000001</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G61" s="58"/>
-      <c r="H61" s="60" t="s">
-        <v>25</v>
-      </c>
-      <c r="I61" s="61">
+        <v>27</v>
+      </c>
+      <c r="G61" s="74"/>
+      <c r="H61" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="I61" s="43">
         <v>22.95</v>
       </c>
     </row>
@@ -2688,36 +2641,36 @@
         <v>4693757.18</v>
       </c>
       <c r="E62" s="5">
-        <v>593.27200000000005</v>
+        <v>590.18700000000001</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G62" s="58"/>
-      <c r="H62" s="60"/>
-      <c r="I62" s="61"/>
+        <v>27</v>
+      </c>
+      <c r="G62" s="74"/>
+      <c r="H62" s="44"/>
+      <c r="I62" s="43"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="23">
         <v>101</v>
       </c>
       <c r="C63" s="19">
-        <v>7510832.6496000001</v>
+        <v>7510832.6459999997</v>
       </c>
       <c r="D63" s="20">
-        <v>4693767.4611</v>
+        <v>4693767.4647000004</v>
       </c>
       <c r="E63" s="5">
-        <v>593.27200000000005</v>
+        <v>590.18700000000001</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G63" s="58"/>
-      <c r="H63" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="I63" s="35">
+        <v>27</v>
+      </c>
+      <c r="G63" s="74"/>
+      <c r="H63" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="I63" s="33">
         <v>20.72</v>
       </c>
     </row>
@@ -2732,31 +2685,29 @@
         <v>4693755.1654000003</v>
       </c>
       <c r="E64" s="15">
-        <v>593.27200000000005</v>
+        <v>590.18700000000001</v>
       </c>
       <c r="F64" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G64" s="59"/>
+        <v>27</v>
+      </c>
+      <c r="G64" s="75"/>
       <c r="H64" s="30" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I64" s="31">
         <f>SUM(I57:I63)</f>
         <v>252.14</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="38"/>
-      <c r="C65" s="38"/>
+    <row r="65" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D65" s="6"/>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
       <c r="G65" s="8"/>
-      <c r="H65" s="39"/>
-      <c r="I65" s="39"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H65" s="9"/>
+      <c r="I65" s="9"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="10" t="s">
         <v>5</v>
       </c>
@@ -2767,188 +2718,201 @@
         <v>1</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G66" s="11" t="s">
         <v>6</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I66" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="23">
         <v>7</v>
       </c>
       <c r="C67" s="19">
-        <v>7510825.8598999996</v>
+        <v>7510823.2538000001</v>
       </c>
       <c r="D67" s="20">
-        <v>4693760.7132999999</v>
+        <v>4693758.1205000002</v>
       </c>
       <c r="E67" s="5">
-        <v>595.572</v>
+        <v>593.27200000000005</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G67" s="72" t="s">
-        <v>38</v>
-      </c>
-      <c r="H67" s="72" t="s">
-        <v>38</v>
-      </c>
-      <c r="I67" s="72">
-        <v>136.41</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="G67" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="H67" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="I67" s="43">
+        <v>208.47</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="23">
         <v>12</v>
       </c>
       <c r="C68" s="19">
-        <v>7510843.0706000002</v>
+        <v>7510843.9336000001</v>
       </c>
       <c r="D68" s="20">
-        <v>4693753.4441</v>
+        <v>4693754.3136</v>
       </c>
       <c r="E68" s="5">
-        <v>595.572</v>
+        <v>593.27200000000005</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G68" s="73"/>
-      <c r="H68" s="73"/>
-      <c r="I68" s="73"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="G68" s="74"/>
+      <c r="H68" s="44"/>
+      <c r="I68" s="43"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="23">
         <v>13</v>
       </c>
       <c r="C69" s="19">
-        <v>7510838.0334000001</v>
+        <v>7510835.4665000001</v>
       </c>
       <c r="D69" s="20">
-        <v>4693748.3690999998</v>
+        <v>4693745.7829</v>
       </c>
       <c r="E69" s="5">
-        <v>595.572</v>
+        <v>593.27200000000005</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G69" s="73"/>
-      <c r="H69" s="73"/>
-      <c r="I69" s="73"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="G69" s="74"/>
+      <c r="H69" s="44"/>
+      <c r="I69" s="43"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="23">
         <v>19</v>
       </c>
       <c r="C70" s="19">
-        <v>7510830.9287</v>
+        <v>7510831.7971999999</v>
       </c>
       <c r="D70" s="20">
-        <v>4693765.7561999997</v>
+        <v>4693766.6201999998</v>
       </c>
       <c r="E70" s="5">
-        <v>595.572</v>
+        <v>593.27200000000005</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G70" s="73"/>
-      <c r="H70" s="73"/>
-      <c r="I70" s="73"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="G70" s="74"/>
+      <c r="H70" s="44"/>
+      <c r="I70" s="43"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="23">
-        <v>105</v>
+        <v>8</v>
       </c>
       <c r="C71" s="19">
-        <v>7510833.7575000003</v>
+        <v>7510834.5362</v>
       </c>
       <c r="D71" s="20">
-        <v>4693752.7050000001</v>
+        <v>4693744.8603999997</v>
       </c>
       <c r="E71" s="5">
-        <v>595.572</v>
+        <v>593.27200000000005</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G71" s="73"/>
-      <c r="H71" s="73"/>
-      <c r="I71" s="73"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="G71" s="74"/>
+      <c r="H71" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="I71" s="43">
+        <v>22.95</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="23">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C72" s="19">
-        <v>7510832.0308999997</v>
+        <v>7510822.3084000004</v>
       </c>
       <c r="D72" s="20">
-        <v>4693751.0022</v>
+        <v>4693757.18</v>
       </c>
       <c r="E72" s="5">
-        <v>595.572</v>
+        <v>593.27200000000005</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G72" s="73"/>
-      <c r="H72" s="73"/>
-      <c r="I72" s="73"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="G72" s="74"/>
+      <c r="H72" s="44"/>
+      <c r="I72" s="43"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="23">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C73" s="19">
-        <v>7510828.3795999996</v>
+        <v>7510832.6496000001</v>
       </c>
       <c r="D73" s="20">
-        <v>4693754.7046999997</v>
+        <v>4693767.4611</v>
       </c>
       <c r="E73" s="5">
-        <v>595.572</v>
+        <v>593.27200000000005</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G73" s="73"/>
-      <c r="H73" s="73"/>
-      <c r="I73" s="73"/>
-    </row>
-    <row r="74" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="G73" s="74"/>
+      <c r="H73" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="I73" s="35">
+        <v>20.72</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="26">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C74" s="27">
-        <v>7510830.1062000003</v>
+        <v>7510844.7790999999</v>
       </c>
       <c r="D74" s="28">
-        <v>4693756.4073999999</v>
+        <v>4693755.1654000003</v>
       </c>
       <c r="E74" s="15">
-        <v>595.572</v>
+        <v>593.27200000000005</v>
       </c>
       <c r="F74" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G74" s="78"/>
-      <c r="H74" s="78"/>
-      <c r="I74" s="78"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="G74" s="75"/>
+      <c r="H74" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="I74" s="31">
+        <f>SUM(I67:I73)</f>
+        <v>252.14</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B75" s="38"/>
       <c r="C75" s="38"/>
       <c r="D75" s="6"/>
@@ -2958,87 +2922,287 @@
       <c r="H75" s="39"/>
       <c r="I75" s="39"/>
     </row>
-    <row r="76" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K76" s="1"/>
-    </row>
-    <row r="77" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A77" s="2" t="s">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B76" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F76" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G76" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H76" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I76" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B77" s="23">
+        <v>7</v>
+      </c>
+      <c r="C77" s="19">
+        <v>7510825.8598999996</v>
+      </c>
+      <c r="D77" s="20">
+        <v>4693760.7132999999</v>
+      </c>
+      <c r="E77" s="5">
+        <v>595.572</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G77" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="H77" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="I77" s="40">
+        <v>136.41</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B78" s="23">
+        <v>12</v>
+      </c>
+      <c r="C78" s="19">
+        <v>7510843.0706000002</v>
+      </c>
+      <c r="D78" s="20">
+        <v>4693753.4441</v>
+      </c>
+      <c r="E78" s="5">
+        <v>595.572</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G78" s="41"/>
+      <c r="H78" s="41"/>
+      <c r="I78" s="41"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B79" s="23">
+        <v>13</v>
+      </c>
+      <c r="C79" s="19">
+        <v>7510838.0334000001</v>
+      </c>
+      <c r="D79" s="20">
+        <v>4693748.3690999998</v>
+      </c>
+      <c r="E79" s="5">
+        <v>595.572</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G79" s="41"/>
+      <c r="H79" s="41"/>
+      <c r="I79" s="41"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B80" s="23">
+        <v>19</v>
+      </c>
+      <c r="C80" s="19">
+        <v>7510830.9287</v>
+      </c>
+      <c r="D80" s="20">
+        <v>4693765.7561999997</v>
+      </c>
+      <c r="E80" s="5">
+        <v>595.572</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G80" s="41"/>
+      <c r="H80" s="41"/>
+      <c r="I80" s="41"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B81" s="23">
+        <v>105</v>
+      </c>
+      <c r="C81" s="19">
+        <v>7510833.7575000003</v>
+      </c>
+      <c r="D81" s="20">
+        <v>4693752.7050000001</v>
+      </c>
+      <c r="E81" s="5">
+        <v>595.572</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G81" s="41"/>
+      <c r="H81" s="41"/>
+      <c r="I81" s="41"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B82" s="23">
+        <v>106</v>
+      </c>
+      <c r="C82" s="19">
+        <v>7510832.0308999997</v>
+      </c>
+      <c r="D82" s="20">
+        <v>4693751.0022</v>
+      </c>
+      <c r="E82" s="5">
+        <v>595.572</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G82" s="41"/>
+      <c r="H82" s="41"/>
+      <c r="I82" s="41"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B83" s="23">
+        <v>107</v>
+      </c>
+      <c r="C83" s="19">
+        <v>7510828.3795999996</v>
+      </c>
+      <c r="D83" s="20">
+        <v>4693754.7046999997</v>
+      </c>
+      <c r="E83" s="5">
+        <v>595.572</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G83" s="41"/>
+      <c r="H83" s="41"/>
+      <c r="I83" s="41"/>
+    </row>
+    <row r="84" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="26">
+        <v>108</v>
+      </c>
+      <c r="C84" s="27">
+        <v>7510830.1062000003</v>
+      </c>
+      <c r="D84" s="28">
+        <v>4693756.4073999999</v>
+      </c>
+      <c r="E84" s="15">
+        <v>595.572</v>
+      </c>
+      <c r="F84" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G84" s="42"/>
+      <c r="H84" s="42"/>
+      <c r="I84" s="42"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B85" s="38"/>
+      <c r="C85" s="38"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="39"/>
+      <c r="I85" s="39"/>
+    </row>
+    <row r="86" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K86" s="1"/>
+    </row>
+    <row r="87" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="49" t="s">
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F77" s="50"/>
-      <c r="G77" s="51"/>
-      <c r="H77" s="45" t="s">
+      <c r="F87" s="66"/>
+      <c r="G87" s="67"/>
+      <c r="H87" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="I77" s="46"/>
-      <c r="J77" s="40"/>
-      <c r="K77" s="41"/>
-    </row>
-    <row r="78" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="52" t="s">
+      <c r="I87" s="62"/>
+      <c r="J87" s="56"/>
+      <c r="K87" s="57"/>
+    </row>
+    <row r="88" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="B78" s="53"/>
-      <c r="C78" s="53"/>
-      <c r="D78" s="54"/>
-      <c r="E78" s="55">
+      <c r="B88" s="69"/>
+      <c r="C88" s="69"/>
+      <c r="D88" s="70"/>
+      <c r="E88" s="71">
         <v>152</v>
       </c>
-      <c r="F78" s="56"/>
-      <c r="G78" s="57"/>
-      <c r="H78" s="47"/>
-      <c r="I78" s="48"/>
-      <c r="J78" s="42"/>
-      <c r="K78" s="43"/>
-    </row>
-    <row r="79" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K79" s="1"/>
-    </row>
-    <row r="80" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K80" s="1"/>
-    </row>
-    <row r="81" spans="11:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K81" s="1"/>
+      <c r="F88" s="72"/>
+      <c r="G88" s="73"/>
+      <c r="H88" s="63"/>
+      <c r="I88" s="64"/>
+      <c r="J88" s="58"/>
+      <c r="K88" s="59"/>
+    </row>
+    <row r="89" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K89" s="1"/>
+    </row>
+    <row r="90" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K90" s="1"/>
+    </row>
+    <row r="91" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K91" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="H67:H74"/>
-    <mergeCell ref="I67:I74"/>
+  <mergeCells count="29">
+    <mergeCell ref="J87:K88"/>
+    <mergeCell ref="A3:K6"/>
+    <mergeCell ref="H87:I88"/>
+    <mergeCell ref="E87:G87"/>
+    <mergeCell ref="A88:D88"/>
+    <mergeCell ref="E88:G88"/>
+    <mergeCell ref="G47:G54"/>
+    <mergeCell ref="G67:G74"/>
+    <mergeCell ref="H67:H70"/>
+    <mergeCell ref="H47:H50"/>
     <mergeCell ref="I47:I50"/>
+    <mergeCell ref="G57:G64"/>
+    <mergeCell ref="H57:H60"/>
     <mergeCell ref="H51:H52"/>
     <mergeCell ref="I51:I52"/>
+    <mergeCell ref="G77:G84"/>
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="C8:J10"/>
+    <mergeCell ref="G15:G32"/>
+    <mergeCell ref="H15:H30"/>
+    <mergeCell ref="I15:I30"/>
+    <mergeCell ref="H77:H84"/>
+    <mergeCell ref="I77:I84"/>
     <mergeCell ref="I57:I60"/>
     <mergeCell ref="H61:H62"/>
     <mergeCell ref="I61:I62"/>
-    <mergeCell ref="A1:K2"/>
-    <mergeCell ref="C8:J10"/>
-    <mergeCell ref="H15:H18"/>
-    <mergeCell ref="I15:I18"/>
-    <mergeCell ref="H19:H21"/>
-    <mergeCell ref="I19:I21"/>
-    <mergeCell ref="G15:G22"/>
-    <mergeCell ref="J77:K78"/>
-    <mergeCell ref="A3:K6"/>
-    <mergeCell ref="H77:I78"/>
-    <mergeCell ref="E77:G77"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="E78:G78"/>
-    <mergeCell ref="G37:G44"/>
-    <mergeCell ref="G57:G64"/>
-    <mergeCell ref="H57:H60"/>
-    <mergeCell ref="H37:H40"/>
-    <mergeCell ref="I37:I40"/>
-    <mergeCell ref="G47:G54"/>
-    <mergeCell ref="H47:H50"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="G67:G74"/>
+    <mergeCell ref="I67:I70"/>
+    <mergeCell ref="H71:H72"/>
+    <mergeCell ref="I71:I72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="58" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>